<commit_message>
Fixed Supp Table S4:
For SBS_set1 and SBS_set2, we showed number of runs of "mSigHdp_ds_3k"
(instead of "mSigHdp") which failed to extract each signature.
</commit_message>
<xml_diff>
--- a/common_code/missed_sig_analysis/New_Table_S4.xlsx
+++ b/common_code/missed_sig_analysis/New_Table_S4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1_main\common_code\missed_sig_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\common_code\missed_sig_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0994862-17FF-4402-A229-F0FF7765E80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814CFE8C-01E3-40A3-8293-226BD961A2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="11925" windowHeight="13860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="495" yWindow="495" windowWidth="16920" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Table S4" sheetId="10" r:id="rId1"/>
@@ -139,15 +139,9 @@
     <t>ID1</t>
   </si>
   <si>
-    <t>Signature missed by both programs in all 5 runs</t>
-  </si>
-  <si>
     <t>Signature missed by SigProfilerExtractor in 4 runs</t>
   </si>
   <si>
-    <t>Signature missed by mSigHdp in all 5 runs</t>
-  </si>
-  <si>
     <t>Remark</t>
   </si>
   <si>
@@ -209,18 +203,6 @@
   </si>
   <si>
     <t>ID10</t>
-  </si>
-  <si>
-    <t>Signature missed by SigProfilerExtractor in 1 runs</t>
-  </si>
-  <si>
-    <t>Signature missed by mSigHdp in 2 runs; Signature missed by SigProfilerExtractor in 4 runs</t>
-  </si>
-  <si>
-    <t>Signature missed by mSigHdp in 2 runs; Signature missed by SigProfilerExtractor in all 5 runs</t>
-  </si>
-  <si>
-    <t>Signature missed by mSigHdp in 1 runs; Signature missed by SigProfilerExtractor in all 5 runs</t>
   </si>
   <si>
     <r>
@@ -235,6 +217,24 @@
       </rPr>
       <t xml:space="preserve"> Table manually edited from output in https://github.com/Rozen-Lab/Liu_et_al_Sup_Files/tree/main/common_code/missed_sig_analysis.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Signature missed by mSigHdp in all 5 runs; Signature missed by SigProfilerExtractor in all 5 runs; </t>
+  </si>
+  <si>
+    <t>Signature missed by mSigHdp in 2 runs</t>
+  </si>
+  <si>
+    <t>Signature missed by mSigHdp in 1 run</t>
+  </si>
+  <si>
+    <t>Signature missed by SigProfilerExtractor in 1 run</t>
+  </si>
+  <si>
+    <t>Signature missed by mSigHdp in all 5 runs; Signature missed by SigProfilerExtractor in all 5 runs</t>
+  </si>
+  <si>
+    <t>Signature missed by mSigHdp in all 5 runs; Signature missed by SigProfilerExtractor in 4 runs</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -479,6 +479,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{25CF7EEA-3B22-47D7-8528-DEF4EA09114D}"/>
@@ -806,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -822,7 +823,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="32"/>
@@ -837,19 +838,19 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="17"/>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="20"/>
       <c r="C4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="16"/>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -863,18 +864,18 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -891,7 +892,7 @@
       <c r="D9" s="5">
         <v>0.94074074074074077</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="33" t="s">
         <v>31</v>
       </c>
     </row>
@@ -905,6 +906,7 @@
       <c r="D10" s="7">
         <v>0.92962962962962958</v>
       </c>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
@@ -916,6 +918,7 @@
       <c r="D11" s="7">
         <v>0.37777777777777777</v>
       </c>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -927,6 +930,7 @@
       <c r="D12" s="7">
         <v>0.33333333333333331</v>
       </c>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
@@ -938,6 +942,7 @@
       <c r="D13" s="7">
         <v>0.32777777777777778</v>
       </c>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
@@ -949,6 +954,7 @@
       <c r="D14" s="7">
         <v>0.28888888888888886</v>
       </c>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
@@ -960,6 +966,7 @@
       <c r="D15" s="7">
         <v>0.2</v>
       </c>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
@@ -971,6 +978,7 @@
       <c r="D16" s="7">
         <v>0.19814814814814816</v>
       </c>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
@@ -982,6 +990,7 @@
       <c r="D17" s="7">
         <v>0.19444444444444445</v>
       </c>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
@@ -993,6 +1002,7 @@
       <c r="D18" s="7">
         <v>0.10555555555555556</v>
       </c>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
@@ -1004,6 +1014,7 @@
       <c r="D19" s="7">
         <v>9.8148148148148151E-2</v>
       </c>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="18" t="s">
@@ -1015,8 +1026,8 @@
       <c r="D20" s="19">
         <v>9.6296296296296297E-2</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>41</v>
+      <c r="E20" s="33" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1029,8 +1040,8 @@
       <c r="D21" s="19">
         <v>9.4444444444444442E-2</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>41</v>
+      <c r="E21" s="33" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1043,6 +1054,7 @@
       <c r="D22" s="7">
         <v>8.7037037037037038E-2</v>
       </c>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
@@ -1054,8 +1066,8 @@
       <c r="D23" s="5">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>40</v>
+      <c r="E23" s="33" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1068,7 +1080,7 @@
       <c r="D24" s="5">
         <v>4.2592592592592592E-2</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="33" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1082,7 +1094,7 @@
       <c r="D25" s="5">
         <v>3.1481481481481478E-2</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="33" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1096,7 +1108,7 @@
       <c r="D26" s="5">
         <v>2.4074074074074074E-2</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="33" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1110,6 +1122,7 @@
       <c r="D27" s="7">
         <v>2.0370370370370372E-2</v>
       </c>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
@@ -1121,19 +1134,20 @@
       <c r="D28" s="7">
         <v>1.6666666666666666E-2</v>
       </c>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="13">
         <v>5</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="12">
         <v>9.2592592592592587E-3</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>31</v>
+      <c r="E29" s="33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1146,7 +1160,7 @@
       <c r="D30" s="5">
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="33" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1160,13 +1174,13 @@
       <c r="D31" s="12">
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>39</v>
+      <c r="E31" s="33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="9"/>
@@ -1213,7 +1227,7 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F35"/>
       <c r="H35"/>
@@ -1255,7 +1269,7 @@
         <v>0.21574074074074101</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F38"/>
       <c r="H38"/>
@@ -1271,7 +1285,7 @@
         <v>0.16574074074074099</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F39"/>
       <c r="H39"/>
@@ -1304,7 +1318,7 @@
     </row>
     <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" s="6">
         <v>53</v>
@@ -1313,7 +1327,7 @@
         <v>4.9074074074074103E-2</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F42"/>
       <c r="H42"/>
@@ -1329,7 +1343,7 @@
         <v>4.81481481481481E-2</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F43"/>
       <c r="H43"/>
@@ -1345,7 +1359,7 @@
         <v>4.72222222222222E-2</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F44"/>
       <c r="H44"/>
@@ -1361,7 +1375,7 @@
         <v>4.6296296296296301E-2</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="F45"/>
       <c r="H45"/>
@@ -1410,7 +1424,7 @@
     </row>
     <row r="49" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" s="6">
         <v>31</v>
@@ -1419,7 +1433,7 @@
         <v>2.87037037037037E-2</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F49"/>
       <c r="H49"/>
@@ -1435,7 +1449,7 @@
         <v>2.4074074074074098E-2</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="F50"/>
       <c r="H50"/>
@@ -1471,7 +1485,7 @@
     </row>
     <row r="53" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C53" s="13">
         <v>20</v>
@@ -1480,14 +1494,14 @@
         <v>1.85185185185185E-2</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F53"/>
       <c r="H53"/>
     </row>
     <row r="54" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C54" s="6">
         <v>15</v>
@@ -1503,7 +1517,7 @@
     </row>
     <row r="55" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C55" s="6">
         <v>13</v>
@@ -1519,7 +1533,7 @@
     </row>
     <row r="56" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C56" s="13">
         <v>12</v>
@@ -1528,7 +1542,7 @@
         <v>1.1111111111111099E-2</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F56"/>
       <c r="H56"/>
@@ -1551,7 +1565,7 @@
     </row>
     <row r="58" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C58" s="30">
         <v>10</v>
@@ -1567,7 +1581,7 @@
     </row>
     <row r="59" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C59" s="13">
         <v>10</v>
@@ -1576,30 +1590,30 @@
         <v>9.2592592592592605E-3</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F59"/>
       <c r="H59"/>
     </row>
     <row r="60" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="30">
+      <c r="C60" s="13">
         <v>8</v>
       </c>
-      <c r="D60" s="31">
+      <c r="D60" s="12">
         <v>7.4074074074074103E-3</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="F60"/>
       <c r="H60"/>
     </row>
     <row r="61" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C61" s="13">
         <v>7</v>
@@ -1608,7 +1622,7 @@
         <v>6.4814814814814804E-3</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F61"/>
       <c r="H61"/>
@@ -1640,7 +1654,7 @@
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F63"/>
       <c r="H63"/>
@@ -1656,14 +1670,14 @@
         <v>1.85185185185185E-3</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="F64"/>
       <c r="H64"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="9"/>
@@ -1814,7 +1828,7 @@
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C77" s="22"/>
       <c r="D77" s="22"/>
@@ -1980,7 +1994,7 @@
     <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C89" s="6">
         <v>51</v>
@@ -1997,7 +2011,7 @@
     <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="27"/>
       <c r="B90" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C90" s="28">
         <v>24</v>

</xml_diff>